<commit_message>
Modifications after debugging and added some functionality/backup solutions
</commit_message>
<xml_diff>
--- a/random.xlsx
+++ b/random.xlsx
@@ -68,14 +68,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -457,474 +454,549 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.453125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.4375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col width="10.5" customWidth="1" style="4" min="1" max="1"/>
-    <col width="10.6" customWidth="1" style="4" min="2" max="3"/>
-    <col width="12.83" customWidth="1" style="4" min="4" max="4"/>
-    <col width="10.6" customWidth="1" style="4" min="5" max="9"/>
+    <col width="10.5" customWidth="1" style="3" min="1" max="1"/>
+    <col width="10.6" customWidth="1" style="3" min="2" max="3"/>
+    <col width="12.83" customWidth="1" style="3" min="4" max="4"/>
+    <col width="10.6" customWidth="1" style="3" min="5" max="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="5">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>vorname</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>pseudonym</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>geburtsdatum</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>alter</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>bdi</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>hy</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>pdq8</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>gruppe</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1" s="5">
-      <c r="A2" s="4" t="inlineStr">
+    <row r="2" ht="12.75" customHeight="1" s="4">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Karl</t>
         </is>
       </c>
-      <c r="B2" s="4" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Fredrickson</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>QqNA3LYg</t>
         </is>
       </c>
-      <c r="D2" s="4" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>10.07.1956</t>
         </is>
       </c>
-      <c r="E2" s="6" t="n">
+      <c r="E2" s="5" t="n">
         <v>67.0007286067933</v>
       </c>
-      <c r="F2" s="6" t="n">
+      <c r="F2" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="n">
+      <c r="G2" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H2" s="6" t="n">
+      <c r="H2" s="5" t="n">
         <v>56</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="5" t="n">
         <v>-1</v>
       </c>
     </row>
-    <row r="3" ht="12.75" customHeight="1" s="5">
-      <c r="A3" s="4" t="inlineStr">
+    <row r="3" ht="12.75" customHeight="1" s="4">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Bobby</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Charlton</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>hdRVvt_!</t>
         </is>
       </c>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>10.07.1956</t>
         </is>
       </c>
-      <c r="E3" s="6" t="n">
+      <c r="E3" s="5" t="n">
         <v>66.9981752424125</v>
       </c>
-      <c r="F3" s="6" t="n">
+      <c r="F3" s="5" t="n">
         <v>45</v>
       </c>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="H3" s="6" t="n">
+      <c r="H3" s="5" t="n">
         <v>67</v>
       </c>
-      <c r="I3" s="6" t="n">
+      <c r="I3" s="5" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1" s="5">
-      <c r="A4" s="4" t="inlineStr">
+    <row r="4" ht="12.75" customHeight="1" s="4">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Adele</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Kramp-Karrenbauer</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>E7FHrrAq</t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>12.04.1976</t>
         </is>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="5" t="n">
         <v>47.2444826616749</v>
       </c>
-      <c r="F4" s="6" t="n">
+      <c r="F4" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="H4" s="5" t="n">
         <v>25</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="5" t="n">
         <v>-1</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" s="5">
-      <c r="A5" s="4" t="inlineStr">
+    <row r="5" ht="15" customHeight="1" s="4">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Amande</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Trotzki</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>UKQ5#P0L</t>
         </is>
       </c>
-      <c r="D5" s="4" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>04.03.1965</t>
         </is>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="5" t="n">
         <v>58.3519453951255</v>
       </c>
-      <c r="F5" s="6" t="n">
+      <c r="F5" s="5" t="n">
         <v>44</v>
       </c>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="5" t="n">
         <v>67</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="5" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" s="5">
-      <c r="A6" s="4" t="inlineStr">
+    <row r="6" ht="15" customHeight="1" s="4">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Guillermo</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>KLaus</t>
         </is>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>rKL##6LD</t>
         </is>
       </c>
-      <c r="D6" s="4" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>01.12.1954</t>
         </is>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="5" t="n">
         <v>68.6079374131979</v>
       </c>
-      <c r="F6" s="6" t="n">
+      <c r="F6" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="5" t="n">
         <v>15</v>
       </c>
-      <c r="I6" s="6" t="n">
+      <c r="I6" s="5" t="n">
         <v>-1</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" s="5">
-      <c r="A7" s="4" t="inlineStr">
+    <row r="7" ht="15" customHeight="1" s="4">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>Luis</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>de Faria</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>6D2vyitk</t>
         </is>
       </c>
-      <c r="D7" s="4" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>18.06.1982</t>
         </is>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="5" t="n">
         <v>41.0624255570879</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G7" s="6" t="n">
+      <c r="G7" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H7" s="6" t="n">
+      <c r="H7" s="5" t="n">
         <v>56</v>
       </c>
-      <c r="I7" s="6" t="n">
+      <c r="I7" s="5" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+    <row r="8" ht="12.75" customHeight="1" s="4">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>Karl</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" s="3" t="inlineStr">
         <is>
           <t>Magnus</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t>qs%2TC§k</t>
         </is>
       </c>
-      <c r="D8" s="4" t="inlineStr">
+      <c r="D8" s="3" t="inlineStr">
         <is>
           <t>14.08.1954</t>
         </is>
       </c>
-      <c r="E8" s="4" t="n">
-        <v>68.90888276557229</v>
-      </c>
-      <c r="F8" s="4" t="n">
+      <c r="E8" s="3" t="n">
+        <v>68.9088827655723</v>
+      </c>
+      <c r="F8" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="G8" s="4" t="n">
+      <c r="G8" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="3" t="n">
         <v>56</v>
       </c>
-      <c r="I8" s="4" t="n">
+      <c r="I8" s="3" t="n">
         <v>-1</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+    <row r="9" ht="12.75" customHeight="1" s="4">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>Fridolin</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>McGyver</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>WI9jXPor</t>
         </is>
       </c>
-      <c r="D9" s="4" t="inlineStr">
+      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>12.06.1943</t>
         </is>
       </c>
-      <c r="E9" s="4" t="n">
-        <v>80.07962661270761</v>
-      </c>
-      <c r="F9" s="4" t="n">
+      <c r="E9" s="3" t="n">
+        <v>80.0796266127076</v>
+      </c>
+      <c r="F9" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="G9" s="4" t="n">
+      <c r="G9" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="H9" s="4" t="n">
+      <c r="H9" s="3" t="n">
         <v>76</v>
       </c>
-      <c r="I9" s="4" t="n">
+      <c r="I9" s="3" t="n">
         <v>-1</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Erna</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="inlineStr">
-        <is>
-          <t>Bert</t>
-        </is>
-      </c>
-      <c r="C10" s="4" t="inlineStr">
-        <is>
-          <t>9!zTYlng</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="inlineStr">
-        <is>
-          <t>24.12.1967</t>
-        </is>
-      </c>
-      <c r="E10" s="4" t="n">
-        <v>55.54574557335919</v>
-      </c>
-      <c r="F10" s="4" t="n">
+    <row r="10" ht="15" customHeight="1" s="4">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>Merta</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Heinrich</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>MPbk5#fk</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>24.01.1963</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>60.4626179880374</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1" s="4">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>de la Vega</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>lKiKNv8Y</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>01.09.1981</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>41.8589330761843</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>67</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" s="4">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>Karl</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Klein</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>0i304HIQ</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>11.01.1981</t>
+        </is>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>42.5064202828192</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="G12" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G10" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="4" t="n">
-        <v>34</v>
-      </c>
-      <c r="I10" s="4" t="n">
+      <c r="H12" s="3" t="n">
+        <v>55</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" ht="12.75" customHeight="1" s="4">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>Anton</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Aberle</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>mOlCfdXq</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>01.01.1965</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>58.5327415836831</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="I13" s="3" t="n">
         <v>-1</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>Merta</t>
-        </is>
-      </c>
-      <c r="B11" s="4" t="inlineStr">
-        <is>
-          <t>Heinrich</t>
-        </is>
-      </c>
-      <c r="C11" s="4" t="inlineStr">
-        <is>
-          <t>MPbk5#fk</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="inlineStr">
-        <is>
-          <t>24.01.1963</t>
-        </is>
-      </c>
-      <c r="E11" s="4" t="n">
-        <v>60.4626179880374</v>
-      </c>
-      <c r="F11" s="4" t="n">
-        <v>24</v>
-      </c>
-      <c r="G11" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="4" t="n">
-        <v>56</v>
-      </c>
-      <c r="I11" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>David</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>de la Vega</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>lKiKNv8Y</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>01.09.1981</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>41.85893307618428</v>
-      </c>
-      <c r="F12" t="n">
-        <v>12</v>
-      </c>
-      <c r="G12" t="n">
-        <v>5</v>
-      </c>
-      <c r="H12" t="n">
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Philipp</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Krämer</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CfQtlfx_</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>28.07.1974</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>48.96501559832272</v>
+      </c>
+      <c r="F14" t="n">
+        <v>45</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" t="n">
         <v>67</v>
       </c>
-      <c r="I12" t="n">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="I14" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="1048576" ht="12.8" customHeight="1" s="4"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>